<commit_message>
add excel files for tc experiment logic refactor
</commit_message>
<xml_diff>
--- a/evaluation/30gb_tc_experiment_ana_executions_and_uptime_difference.xlsx
+++ b/evaluation/30gb_tc_experiment_ana_executions_and_uptime_difference.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fschnei4/TUB_Master_ISM/SoSe21/MA/msc-thesis-saft-experiments/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB27C8F2-2673-8448-8F5E-7F374B509A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25019C9-5B73-AE4C-B5AB-323C6FF7DF83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6560" yWindow="29260" windowWidth="35840" windowHeight="20940" xr2:uid="{6E3BB99E-08A2-F943-AD06-C2CEE3AB35A4}"/>
+    <workbookView xWindow="24480" yWindow="29260" windowWidth="17920" windowHeight="20940" xr2:uid="{6E3BB99E-08A2-F943-AD06-C2CEE3AB35A4}"/>
   </bookViews>
   <sheets>
     <sheet name="App level" sheetId="1" r:id="rId1"/>
     <sheet name="Job level" sheetId="2" r:id="rId2"/>
     <sheet name="Stage level" sheetId="3" r:id="rId3"/>
-    <sheet name="Task level" sheetId="4" r:id="rId4"/>
+    <sheet name="Task level (too detailed)" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>